<commit_message>
Created list of pages, edited a few small things
</commit_message>
<xml_diff>
--- a/Page Details and Checklist.xlsx
+++ b/Page Details and Checklist.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CIS2261_Team_Talent2.0_FP\CIS2261_Team_Talent_FP_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B79F951-754E-426C-B4FA-6AA5B4319754}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B6A0AD-C9F5-4574-8328-2BCAC682123A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{304D8678-0BEF-4E4F-B0F9-10C786B92F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>Logout Option</t>
   </si>
@@ -42,22 +43,13 @@
     <t>Authentication</t>
   </si>
   <si>
-    <t>Home Page</t>
-  </si>
-  <si>
     <t>Add User</t>
   </si>
   <si>
-    <t>Confirm user details</t>
-  </si>
-  <si>
     <t>show confirmation and details</t>
   </si>
   <si>
     <t>give option to add another user</t>
-  </si>
-  <si>
-    <t>give option to add the user as a student?  What about parent/educator etc?</t>
   </si>
   <si>
     <t>Add Student</t>
@@ -197,8 +189,154 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Authentication levels, session with user ID and access level &amp; CSS applied to it</t>
+      <t xml:space="preserve"> Authentication levels, session to get user ID and access level of logged in user &amp; CSS applied to it</t>
     </r>
+  </si>
+  <si>
+    <t>Home page needs to be created</t>
+  </si>
+  <si>
+    <t>Menu links need to be working</t>
+  </si>
+  <si>
+    <t>Add user page, remove user id</t>
+  </si>
+  <si>
+    <t>Add user confirm page needs to be made</t>
+  </si>
+  <si>
+    <t>Add user confirmation page needs confirmation of details added, link to add a "type of user" and  cleaned up</t>
+  </si>
+  <si>
+    <t>pop-up Confirm user details</t>
+  </si>
+  <si>
+    <t>remove user id from form</t>
+  </si>
+  <si>
+    <t>On navbar &amp; linked</t>
+  </si>
+  <si>
+    <t>prevent "backdoor"entry</t>
+  </si>
+  <si>
+    <t>show confirmation and details and give option to add the user as a student?  What about parent/educator etc?</t>
+  </si>
+  <si>
+    <t>On navbar &amp; linked?  Or not because it happens after add user?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Most pages need: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Validation in place, place on navbar, preventative measures for backdoor entry</t>
+    </r>
+  </si>
+  <si>
+    <t>Delete Parent</t>
+  </si>
+  <si>
+    <t>Delete Student</t>
+  </si>
+  <si>
+    <t>Delete User</t>
+  </si>
+  <si>
+    <t>Edit Parent</t>
+  </si>
+  <si>
+    <t>Edit Student</t>
+  </si>
+  <si>
+    <t>Edit User</t>
+  </si>
+  <si>
+    <t>Login_base</t>
+  </si>
+  <si>
+    <t>setCookie</t>
+  </si>
+  <si>
+    <t>ajax</t>
+  </si>
+  <si>
+    <t>Display Report Card</t>
+  </si>
+  <si>
+    <t>Display School Subject Average</t>
+  </si>
+  <si>
+    <t>Display Student Subject history</t>
+  </si>
+  <si>
+    <t>Enter Mark</t>
+  </si>
+  <si>
+    <t>Get Student Enter Mark</t>
+  </si>
+  <si>
+    <t>Request Report Card</t>
+  </si>
+  <si>
+    <t>Request School Subject Average</t>
+  </si>
+  <si>
+    <t>Request Student Subject Averave</t>
+  </si>
+  <si>
+    <t>View IEP</t>
+  </si>
+  <si>
+    <t>Index/Home Page</t>
+  </si>
+  <si>
+    <t>NavBar</t>
+  </si>
+  <si>
+    <t>Logout if logged in</t>
+  </si>
+  <si>
+    <t>Login if logged out</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Resize to bring fields closer together and less empty space/smaller 'box'</t>
+  </si>
+  <si>
+    <t>Navbar For all:</t>
+  </si>
+  <si>
+    <t>NavBar Specific:</t>
+  </si>
+  <si>
+    <t>CSS Suggestions</t>
+  </si>
+  <si>
+    <t>***Should we do this as an includes?***</t>
   </si>
 </sst>
 </file>
@@ -268,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,6 +422,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,23 +742,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18450B75-F9C6-4800-9252-7DA470FB3294}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
     <col min="7" max="7" width="20.26953125" customWidth="1"/>
     <col min="8" max="8" width="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D1" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -623,13 +768,13 @@
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -645,273 +790,555 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D4" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D6" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D7" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D10" s="1" t="s">
-        <v>3</v>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D13" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D14" s="3" t="s">
-        <v>4</v>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D15" s="4" t="s">
-        <v>11</v>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="4" t="s">
-        <v>12</v>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D19" s="2" t="s">
-        <v>29</v>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D20" s="2" t="s">
-        <v>6</v>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D21" s="2" t="s">
-        <v>7</v>
+      <c r="D21" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D22" s="2" t="s">
-        <v>8</v>
+      <c r="D22" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D23" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D24" s="1" t="s">
-        <v>9</v>
+      <c r="D24" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D25" s="4" t="s">
-        <v>11</v>
+      <c r="D25" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D26" s="4" t="s">
-        <v>22</v>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D27" s="4" t="s">
-        <v>13</v>
+      <c r="D27" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D28" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D29" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D30" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D31" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D32" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D34" s="1" t="s">
-        <v>10</v>
+      <c r="D34" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D35" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D37" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D36" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D37" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D38" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D39" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D40" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D41" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D42" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D43" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D44" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D45" s="4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D46" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D47" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D48" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D50" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D51" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D52" s="1" t="s">
-        <v>21</v>
+      <c r="D52" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D53" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D54" s="4" t="s">
-        <v>23</v>
+      <c r="D54" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D55" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D56" s="2" t="s">
-        <v>34</v>
+      <c r="D56" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D58" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D59" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D61" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D63" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D65" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D67" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D69" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D71" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D73" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D75" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D77" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D79" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D81" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D83" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D85" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D87" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D89" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D91" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D99" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D100" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D101" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D58" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D59" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D60" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D61" s="2" t="s">
-        <v>34</v>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D102" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D103" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D104" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D105" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D106" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D107" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D108" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D111" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D112" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D113" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D114" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D115" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D116" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D117" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D118" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D120" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D123" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6149A0B4-AD29-4981-ACB8-3AA7FF16B4D3}">
+  <dimension ref="D2:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="4:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="4:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes and fixes to Student subject history files.
</commit_message>
<xml_diff>
--- a/Page Details and Checklist.xlsx
+++ b/Page Details and Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CIS2261_Team_Talent2.0_FP\CIS2261_Team_Talent_FP_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\CIS2261_Team_Talent_FP_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B6A0AD-C9F5-4574-8328-2BCAC682123A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D46B47-A4B8-4E36-B406-1BD077D14139}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{304D8678-0BEF-4E4F-B0F9-10C786B92F8F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
   <si>
     <t>Logout Option</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>***Should we do this as an includes?***</t>
+  </si>
+  <si>
+    <t>Added semester number to display (JG - 2018/02/03)</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,6 +430,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,22 +748,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18450B75-F9C6-4800-9252-7DA470FB3294}">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
@@ -766,7 +772,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -781,509 +787,514 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D81" s="3" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D83" s="3" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D85" s="3" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D87" s="3" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D89" s="3" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D91" s="3" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D99" s="1" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D100" s="4" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D101" s="4" t="s">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D102" s="4" t="s">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D103" s="2" t="s">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D104" s="1" t="s">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D105" s="4" t="s">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D106" s="4" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D107" s="4" t="s">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D108" s="2" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D111" s="3" t="s">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D112" s="3" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D113" s="10" t="s">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D114" s="9" t="s">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D115" s="9" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D116" s="9" t="s">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D117" s="9" t="s">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D118" s="9" t="s">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D120" s="10" t="s">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D123" s="1" t="s">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1301,39 +1312,39 @@
       <selection activeCell="D9" sqref="D9:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="4:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Code changes. Authentication for Request Report Card about complete.
</commit_message>
<xml_diff>
--- a/Page Details and Checklist.xlsx
+++ b/Page Details and Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CIS2261_Team_Talent2.0_FP\CIS2261_Team_Talent_FP_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgaudet109873\Documents\GitHub\CIS2261_Team_Talent_FP_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D557E0A4-4E03-435B-9C01-C4F6A1F3CCC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3B503E-1E50-4F6B-9065-91C6B02C171B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{304D8678-0BEF-4E4F-B0F9-10C786B92F8F}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{304D8678-0BEF-4E4F-B0F9-10C786B92F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t>Logout Option</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Authenticate</t>
   </si>
   <si>
-    <t>Request Student Subject Average</t>
-  </si>
-  <si>
     <t>put reset button on it to clear form if needed.</t>
   </si>
   <si>
@@ -393,6 +390,12 @@
   </si>
   <si>
     <t>show confirmation and details and give option to add the user as a student?  Confirmation Needs to be CSS'd!!! What about if adding parent or ecucator?</t>
+  </si>
+  <si>
+    <t>JG</t>
+  </si>
+  <si>
+    <t>Request Student Subject History</t>
   </si>
 </sst>
 </file>
@@ -878,21 +881,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18450B75-F9C6-4800-9252-7DA470FB3294}">
   <dimension ref="A1:XFD153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="99.26953125" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="99.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="5" t="s">
         <v>26</v>
       </c>
@@ -901,7 +904,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -916,7 +919,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
         <v>72</v>
       </c>
@@ -925,7 +928,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>73</v>
       </c>
@@ -934,7 +937,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="16" t="s">
         <v>74</v>
       </c>
@@ -943,223 +946,223 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D51" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -17542,433 +17545,439 @@
       <c r="XFC52" s="2"/>
       <c r="XFD52" s="2"/>
     </row>
-    <row r="53" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D56" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D57" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D58" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D63" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D64" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D67" s="22" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D68" s="22" t="s">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D69" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D84" s="2" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D85" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D89" s="11" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D90" s="11" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D91" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="11"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D101" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D106" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D107" s="23" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>99</v>
+      </c>
+      <c r="D107" s="26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D111" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D112" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D113" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D117" s="3" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>99</v>
+      </c>
       <c r="D118" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D119" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D122" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D123" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D124" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D125" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="4:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D128" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D129" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D130" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D131" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D132" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D133" s="20"/>
     </row>
-    <row r="134" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D134" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D135" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D136" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D137" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D138" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D141" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D142" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D143" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D144" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153" s="1"/>
     </row>
   </sheetData>
@@ -17985,24 +17994,24 @@
       <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -18021,75 +18030,75 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="143.90625" customWidth="1"/>
+    <col min="1" max="1" width="143.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Code changes. View IEP is locked down.
</commit_message>
<xml_diff>
--- a/Page Details and Checklist.xlsx
+++ b/Page Details and Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgaudet109873\Documents\GitHub\CIS2261_Team_Talent_FP_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgaudet109873\CIS2261_Team_Talent_FP_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3B503E-1E50-4F6B-9065-91C6B02C171B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4CB9C9-36E8-4C1D-BD58-CAAFF9196ADD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{304D8678-0BEF-4E4F-B0F9-10C786B92F8F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Logout Option</t>
   </si>
@@ -397,6 +397,15 @@
   <si>
     <t>Request Student Subject History</t>
   </si>
+  <si>
+    <t>Reset Btn??</t>
+  </si>
+  <si>
+    <t>Search Student</t>
+  </si>
+  <si>
+    <t>Should this be an Admin only function?? Only option is to edit the student once a search is complete.</t>
+  </si>
 </sst>
 </file>
 
@@ -496,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,6 +572,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -879,17 +895,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18450B75-F9C6-4800-9252-7DA470FB3294}">
-  <dimension ref="A1:XFD153"/>
+  <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="99.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="51" customWidth="1"/>
@@ -992,152 +1008,158 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
       <c r="D28" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D30" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D33" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
       <c r="D35" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" s="22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="22" t="s">
         <v>4</v>
       </c>
@@ -17592,393 +17614,412 @@
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="D63" s="3" t="s">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="D64" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="D64" s="4" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="22" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="2"/>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="3" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="2"/>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="3" t="s">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="23" t="s">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="22" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="2"/>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="3"/>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="2"/>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="3" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="25" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="25" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="3" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="26" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="11" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="11" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="11" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="11"/>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="11"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="2"/>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="3" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="26" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="3"/>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="3"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D101" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D99" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="2"/>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="3" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="3"/>
-    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="2"/>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>99</v>
       </c>
-      <c r="D107" s="26" t="s">
+      <c r="D110" s="26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="2" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="3"/>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="2"/>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="3" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="25" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="2" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="3"/>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="3"/>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="3"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="2"/>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="3" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>99</v>
       </c>
-      <c r="D118" s="25" t="s">
+      <c r="D121" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="2" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="3"/>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="2"/>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="3" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="25" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="2" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="2" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="2"/>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="2"/>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="2"/>
     </row>
-    <row r="128" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D128" s="18" t="s">
+    <row r="131" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D131" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
+    <row r="132" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D129" s="19" t="s">
+      <c r="D132" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D130" s="19" t="s">
+    <row r="133" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D133" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D131" s="19" t="s">
+    <row r="134" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D132" s="20" t="s">
+    <row r="135" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D133" s="20"/>
+    <row r="136" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="20"/>
     </row>
-    <row r="134" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D134" s="18" t="s">
+    <row r="137" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D135" s="19" t="s">
+    <row r="138" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D136" s="19" t="s">
+    <row r="139" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D137" s="19" t="s">
+    <row r="140" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D138" s="20" t="s">
+    <row r="141" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D141" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="3" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="3" t="s">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="10" t="s">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="10" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" s="10" t="s">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="1"/>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>